<commit_message>
Update banco de dados
</commit_message>
<xml_diff>
--- a/docs/Tabela Pert CPM.xlsx
+++ b/docs/Tabela Pert CPM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desenvolvimento\Desktop\EPONA\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78B61C7E-3A1B-491A-8E26-B7713A3D1211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31663E76-67A9-4821-8F1C-CBC1FCC5543A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{3AF43CE9-10C3-4725-893B-917E4B446930}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{3AF43CE9-10C3-4725-893B-917E4B446930}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>A</t>
   </si>
@@ -92,14 +92,20 @@
     <t>4,5,7</t>
   </si>
   <si>
-    <t>4,5,11</t>
+    <t>4,5,7,8,9</t>
+  </si>
+  <si>
+    <t>I,H</t>
+  </si>
+  <si>
+    <t>8,9,10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +115,14 @@
     </font>
     <font>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -156,7 +170,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECD6EB6-B084-403E-B9CE-9AD1F7264B17}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,10 +516,10 @@
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -515,11 +529,11 @@
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -527,11 +541,11 @@
       <c r="C2" s="2">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -539,11 +553,11 @@
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -551,11 +565,11 @@
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -563,11 +577,11 @@
       <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -577,11 +591,11 @@
       <c r="C6" s="2">
         <v>3</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -589,11 +603,12 @@
       <c r="C7" s="2">
         <v>7</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -603,11 +618,11 @@
       <c r="C8" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -617,11 +632,11 @@
       <c r="C9" s="2">
         <v>3</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>7.8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -631,37 +646,37 @@
       <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C11" s="2">
         <v>10</v>
       </c>
-      <c r="D11" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="2">
         <v>3</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D12" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -669,7 +684,7 @@
       <c r="C13" s="2">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>12</v>
       </c>
     </row>
@@ -680,6 +695,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003B6751EEBFA44B458FA51DB47910BAC9" ma:contentTypeVersion="0" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="466a1584243eed19cc31385f3980d601">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7be11120535bb6d6d405ec987f01af38">
     <xsd:element name="properties">
@@ -793,22 +823,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AD1C02C-8BF7-402B-894A-FAB9310A2001}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFCAAF37-27F0-4333-9481-17635687C38C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541DD091-09CC-4F23-8F8F-E043F0859C07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -822,27 +860,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFCAAF37-27F0-4333-9481-17635687C38C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AD1C02C-8BF7-402B-894A-FAB9310A2001}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>